<commit_message>
Dispatcher added to Initialization state and init application done successfully with orchestrator credential.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/FrameworkTemplates/REFramework/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REFramework\Automate_UIApplication\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC1C4FA-CCD2-444F-9125-8E3B25E920F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -159,7 +159,28 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>UIDemoQueue</t>
+  </si>
+  <si>
+    <t>Data\Transactions.xlsx</t>
+  </si>
+  <si>
+    <t>Application path</t>
+  </si>
+  <si>
+    <t>UIDemoApplication_Path</t>
+  </si>
+  <si>
+    <t>UIDemoTransactionData_Path</t>
+  </si>
+  <si>
+    <t>Input_SheetName</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>UIDemo\UIDemo.exe</t>
   </si>
 </sst>
 </file>
@@ -535,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -594,31 +615,61 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:26" ht="43.2">
+      <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
-      <c r="A5" t="s">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="28.8">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1608,6 +1659,10 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>